<commit_message>
Added keep doing and avoid doing
Added keep doing and avoid doing
</commit_message>
<xml_diff>
--- a/Team Report_Rafif, Maha, Saloni-Final.xlsx
+++ b/Team Report_Rafif, Maha, Saloni-Final.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27510"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafifarab/Desktop/SSW-555-GEDCOM/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -16,13 +21,13 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId7"/>
     <sheet name="Stories" sheetId="11" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -686,9 +691,6 @@
     <t xml:space="preserve">Meeting twice every week. </t>
   </si>
   <si>
-    <t>Missing deadlines</t>
-  </si>
-  <si>
     <t>Commiting progress to github</t>
   </si>
   <si>
@@ -759,6 +761,9 @@
   </si>
   <si>
     <t>if less than # months print Name</t>
+  </si>
+  <si>
+    <t>Avoid delay</t>
   </si>
 </sst>
 </file>
@@ -1073,11 +1078,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2073009976"/>
-        <c:axId val="2073013048"/>
+        <c:axId val="764616320"/>
+        <c:axId val="764620272"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2073009976"/>
+        <c:axId val="764616320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1087,14 +1092,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073013048"/>
+        <c:crossAx val="764620272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2073013048"/>
+        <c:axId val="764620272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1105,7 +1110,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073009976"/>
+        <c:crossAx val="764616320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1483,15 +1488,15 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="5" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -1508,7 +1513,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>159</v>
       </c>
@@ -1525,7 +1530,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>160</v>
       </c>
@@ -1542,7 +1547,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -1559,7 +1564,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>29</v>
       </c>
@@ -1579,11 +1584,6 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1595,33 +1595,33 @@
       <selection activeCell="B37" sqref="B37:E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1635,10 +1635,10 @@
         <v>159</v>
       </c>
       <c r="E2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>116</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>118</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>119</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>120</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1701,10 +1701,10 @@
         <v>160</v>
       </c>
       <c r="E8" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>122</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>123</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>124</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>125</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>126</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>127</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>128</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>129</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>131</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>132</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>133</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>134</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B22" t="s">
         <v>135</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
         <v>138</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
         <v>139</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
         <v>140</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1897,10 +1897,10 @@
         <v>159</v>
       </c>
       <c r="E28" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B29" t="s">
         <v>142</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1922,10 +1922,10 @@
         <v>160</v>
       </c>
       <c r="E30" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>144</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>145</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B33" t="s">
         <v>146</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B34" t="s">
         <v>147</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B35" t="s">
         <v>148</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
         <v>149</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B38" t="s">
         <v>151</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>2</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
         <v>153</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B41" t="s">
         <v>154</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B42" t="s">
         <v>155</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B43" t="s">
         <v>156</v>
       </c>
@@ -2051,11 +2051,6 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2067,17 +2062,17 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="2"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2097,7 +2092,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>40442</v>
       </c>
@@ -2108,7 +2103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>40455</v>
       </c>
@@ -2135,11 +2130,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2147,25 +2137,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="6"/>
-    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="6"/>
+    <col min="11" max="11" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2194,7 +2184,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>115</v>
       </c>
@@ -2205,7 +2195,7 @@
         <v>159</v>
       </c>
       <c r="D2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -2220,10 +2210,10 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>184</v>
       </c>
@@ -2231,7 +2221,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>185</v>
       </c>
@@ -2239,10 +2229,10 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="14"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>117</v>
       </c>
@@ -2262,10 +2252,10 @@
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>178</v>
       </c>
@@ -2273,7 +2263,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>180</v>
       </c>
@@ -2281,7 +2271,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>182</v>
       </c>
@@ -2289,7 +2279,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>121</v>
       </c>
@@ -2300,7 +2290,7 @@
         <v>160</v>
       </c>
       <c r="D13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E13">
         <v>100</v>
@@ -2315,11 +2305,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
         <v>188</v>
       </c>
@@ -2327,7 +2317,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
         <v>189</v>
       </c>
@@ -2335,7 +2325,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="26">
+    <row r="17" spans="1:8" ht="39" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
         <v>200</v>
       </c>
@@ -2343,7 +2333,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="26">
+    <row r="18" spans="1:8" ht="39" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
         <v>201</v>
       </c>
@@ -2351,10 +2341,10 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>137</v>
       </c>
@@ -2374,11 +2364,11 @@
         <v>240</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="14" t="s">
         <v>195</v>
       </c>
@@ -2386,7 +2376,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="14" t="s">
         <v>196</v>
       </c>
@@ -2394,7 +2384,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="26">
+    <row r="24" spans="1:8" ht="26" x14ac:dyDescent="0.15">
       <c r="A24" s="14" t="s">
         <v>197</v>
       </c>
@@ -2402,11 +2392,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>141</v>
       </c>
@@ -2417,7 +2407,7 @@
         <v>159</v>
       </c>
       <c r="D26" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E26">
         <v>100</v>
@@ -2432,11 +2422,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="4"/>
       <c r="B27"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" s="14" t="s">
         <v>191</v>
       </c>
@@ -2444,11 +2434,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" s="14"/>
       <c r="B29"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>143</v>
       </c>
@@ -2459,7 +2449,7 @@
         <v>160</v>
       </c>
       <c r="D30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E30">
         <v>100</v>
@@ -2474,11 +2464,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31" s="4"/>
       <c r="B31"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32" s="14" t="s">
         <v>204</v>
       </c>
@@ -2486,7 +2476,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="14" t="s">
         <v>207</v>
       </c>
@@ -2494,48 +2484,43 @@
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B35" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B37" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B38" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B41" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2543,16 +2528,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2581,7 +2566,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>130</v>
       </c>
@@ -2601,23 +2586,23 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="B5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>136</v>
       </c>
@@ -2637,23 +2622,23 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" t="s">
         <v>215</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" s="14" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="14" t="s">
+      <c r="B10" t="s">
         <v>217</v>
       </c>
-      <c r="B10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>150</v>
       </c>
@@ -2673,31 +2658,31 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
         <v>227</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>228</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>231</v>
       </c>
-      <c r="B17" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>152</v>
       </c>
@@ -2717,31 +2702,26 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
+        <v>218</v>
+      </c>
+      <c r="B21" t="s">
         <v>219</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>221</v>
-      </c>
-      <c r="B22" t="s">
-        <v>222</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2753,9 +2733,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2787,11 +2767,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2803,9 +2778,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2837,11 +2812,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2853,13 +2823,13 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>114</v>
       </c>
@@ -2870,7 +2840,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
+    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -2881,7 +2851,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -2892,7 +2862,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -2903,7 +2873,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -2914,7 +2884,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -2925,7 +2895,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -2936,7 +2906,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45">
+    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -2947,7 +2917,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -2958,7 +2928,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -2969,7 +2939,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15">
+    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -2980,7 +2950,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15">
+    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -2991,7 +2961,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30">
+    <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -3002,7 +2972,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30">
+    <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -3013,7 +2983,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15">
+    <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -3024,7 +2994,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>129</v>
       </c>
@@ -3035,7 +3005,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15">
+    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>130</v>
       </c>
@@ -3046,7 +3016,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>131</v>
       </c>
@@ -3057,7 +3027,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>132</v>
       </c>
@@ -3068,7 +3038,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -3079,7 +3049,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15">
+    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>134</v>
       </c>
@@ -3090,7 +3060,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30">
+    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>135</v>
       </c>
@@ -3101,7 +3071,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30">
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>136</v>
       </c>
@@ -3112,7 +3082,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30">
+    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>137</v>
       </c>
@@ -3123,7 +3093,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30">
+    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>138</v>
       </c>
@@ -3134,7 +3104,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30">
+    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>139</v>
       </c>
@@ -3145,7 +3115,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="60">
+    <row r="27" spans="1:3" ht="80" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>140</v>
       </c>
@@ -3156,7 +3126,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>141</v>
       </c>
@@ -3167,7 +3137,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15">
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>142</v>
       </c>
@@ -3178,7 +3148,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -3189,7 +3159,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>144</v>
       </c>
@@ -3200,7 +3170,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30">
+    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -3211,7 +3181,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>146</v>
       </c>
@@ -3222,7 +3192,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30">
+    <row r="34" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>147</v>
       </c>
@@ -3233,7 +3203,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30">
+    <row r="35" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>148</v>
       </c>
@@ -3244,7 +3214,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30">
+    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>149</v>
       </c>
@@ -3255,7 +3225,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15">
+    <row r="37" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>150</v>
       </c>
@@ -3266,7 +3236,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30">
+    <row r="38" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -3277,7 +3247,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30">
+    <row r="39" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>152</v>
       </c>
@@ -3288,7 +3258,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30">
+    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>153</v>
       </c>
@@ -3299,7 +3269,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30">
+    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>154</v>
       </c>
@@ -3310,7 +3280,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15">
+    <row r="42" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>155</v>
       </c>
@@ -3321,7 +3291,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30">
+    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>156</v>
       </c>
@@ -3335,10 +3305,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating sprint 1 and 2
updating sprint 1 and 2
</commit_message>
<xml_diff>
--- a/Team Report_Rafif, Maha, Saloni-Final.xlsx
+++ b/Team Report_Rafif, Maha, Saloni-Final.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26207"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salonisetia/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -16,20 +21,17 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId7"/>
     <sheet name="Stories" sheetId="11" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="245">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -759,6 +761,42 @@
   </si>
   <si>
     <t>Avoid delay</t>
+  </si>
+  <si>
+    <t>T02.01</t>
+  </si>
+  <si>
+    <t>Find their birth date</t>
+  </si>
+  <si>
+    <t>Find their marriage date</t>
+  </si>
+  <si>
+    <t>T02.02</t>
+  </si>
+  <si>
+    <t>T02.03</t>
+  </si>
+  <si>
+    <t>T02.04</t>
+  </si>
+  <si>
+    <t>T10.01</t>
+  </si>
+  <si>
+    <t>Find married Individuals</t>
+  </si>
+  <si>
+    <t>Check if marriage date is after 14 years of birth</t>
+  </si>
+  <si>
+    <t>Check if birth happens before marriage</t>
+  </si>
+  <si>
+    <t>T10.02</t>
+  </si>
+  <si>
+    <t>T10.03</t>
   </si>
 </sst>
 </file>
@@ -1077,11 +1115,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2130346040"/>
-        <c:axId val="2130349128"/>
+        <c:axId val="-2119494336"/>
+        <c:axId val="-2119491408"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2130346040"/>
+        <c:axId val="-2119494336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,14 +1129,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130349128"/>
+        <c:crossAx val="-2119491408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2130349128"/>
+        <c:axId val="-2119491408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1109,7 +1147,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130346040"/>
+        <c:crossAx val="-2119494336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1487,15 +1525,15 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="5" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -1512,7 +1550,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>159</v>
       </c>
@@ -1529,7 +1567,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>160</v>
       </c>
@@ -1546,7 +1584,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -1563,7 +1601,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>29</v>
       </c>
@@ -1583,11 +1621,6 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1595,20 +1628,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37:E37"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>210</v>
       </c>
@@ -1625,7 +1658,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1642,15 +1675,24 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>116</v>
       </c>
       <c r="C3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="D3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1664,10 +1706,10 @@
         <v>161</v>
       </c>
       <c r="E4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>118</v>
       </c>
@@ -1675,7 +1717,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>119</v>
       </c>
@@ -1683,7 +1725,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>120</v>
       </c>
@@ -1691,7 +1733,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1708,7 +1750,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>122</v>
       </c>
@@ -1716,7 +1758,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>123</v>
       </c>
@@ -1724,15 +1766,24 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>2</v>
+      </c>
       <c r="B11" t="s">
         <v>124</v>
       </c>
       <c r="C11" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="D11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>125</v>
       </c>
@@ -1740,7 +1791,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>126</v>
       </c>
@@ -1748,7 +1799,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>127</v>
       </c>
@@ -1756,7 +1807,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>128</v>
       </c>
@@ -1764,7 +1815,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>129</v>
       </c>
@@ -1772,7 +1823,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1789,7 +1840,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>131</v>
       </c>
@@ -1797,7 +1848,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>132</v>
       </c>
@@ -1805,7 +1856,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>133</v>
       </c>
@@ -1813,7 +1864,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>134</v>
       </c>
@@ -1821,7 +1872,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B22" t="s">
         <v>135</v>
       </c>
@@ -1829,7 +1880,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1846,7 +1897,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1860,10 +1911,10 @@
         <v>161</v>
       </c>
       <c r="E24" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
         <v>138</v>
       </c>
@@ -1871,7 +1922,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
         <v>139</v>
       </c>
@@ -1879,7 +1930,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
         <v>140</v>
       </c>
@@ -1887,7 +1938,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1904,7 +1955,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B29" t="s">
         <v>142</v>
       </c>
@@ -1912,7 +1963,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1929,7 +1980,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>144</v>
       </c>
@@ -1937,7 +1988,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>145</v>
       </c>
@@ -1945,7 +1996,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B33" t="s">
         <v>146</v>
       </c>
@@ -1953,7 +2004,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B34" t="s">
         <v>147</v>
       </c>
@@ -1961,7 +2012,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B35" t="s">
         <v>148</v>
       </c>
@@ -1969,7 +2020,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
         <v>149</v>
       </c>
@@ -1977,7 +2028,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1994,7 +2045,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B38" t="s">
         <v>151</v>
       </c>
@@ -2002,7 +2053,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>2</v>
       </c>
@@ -2019,7 +2070,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
         <v>153</v>
       </c>
@@ -2027,7 +2078,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B41" t="s">
         <v>154</v>
       </c>
@@ -2035,7 +2086,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B42" t="s">
         <v>155</v>
       </c>
@@ -2043,7 +2094,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B43" t="s">
         <v>156</v>
       </c>
@@ -2055,11 +2106,6 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2067,21 +2113,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="2"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2101,7 +2147,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>40440</v>
       </c>
@@ -2121,7 +2167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>40454</v>
       </c>
@@ -2148,11 +2194,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2160,25 +2201,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView topLeftCell="A11" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="6"/>
-    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="6"/>
+    <col min="11" max="11" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2207,7 +2248,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>115</v>
       </c>
@@ -2236,10 +2277,10 @@
         <v>41182</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>184</v>
       </c>
@@ -2247,7 +2288,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>185</v>
       </c>
@@ -2255,10 +2296,10 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="14"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>117</v>
       </c>
@@ -2277,11 +2318,20 @@
       <c r="F7">
         <v>240</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+      <c r="I7" s="6">
+        <v>41184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>178</v>
       </c>
@@ -2289,7 +2339,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>180</v>
       </c>
@@ -2297,7 +2347,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>182</v>
       </c>
@@ -2305,7 +2355,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>121</v>
       </c>
@@ -2334,11 +2384,11 @@
         <v>41181</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
         <v>188</v>
       </c>
@@ -2346,7 +2396,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
         <v>189</v>
       </c>
@@ -2354,7 +2404,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="26">
+    <row r="17" spans="1:9" ht="39" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
         <v>200</v>
       </c>
@@ -2362,7 +2412,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="26">
+    <row r="18" spans="1:9" ht="39" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
         <v>201</v>
       </c>
@@ -2370,10 +2420,10 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>137</v>
       </c>
@@ -2392,12 +2442,21 @@
       <c r="F20">
         <v>240</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="G20">
+        <v>17</v>
+      </c>
+      <c r="H20">
+        <v>40</v>
+      </c>
+      <c r="I20" s="6">
+        <v>41184</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="14" t="s">
         <v>195</v>
       </c>
@@ -2405,7 +2464,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="14" t="s">
         <v>196</v>
       </c>
@@ -2413,7 +2472,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="26">
+    <row r="24" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A24" s="14" t="s">
         <v>197</v>
       </c>
@@ -2421,11 +2480,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>141</v>
       </c>
@@ -2454,11 +2513,11 @@
         <v>41184</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="4"/>
       <c r="B27"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="14" t="s">
         <v>191</v>
       </c>
@@ -2466,11 +2525,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="14"/>
       <c r="B29"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>143</v>
       </c>
@@ -2499,11 +2558,11 @@
         <v>41184</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="4"/>
       <c r="B31"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="14" t="s">
         <v>204</v>
       </c>
@@ -2511,7 +2570,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="14" t="s">
         <v>207</v>
       </c>
@@ -2519,35 +2578,35 @@
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B35" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B37" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B38" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B41" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
         <v>232</v>
       </c>
@@ -2556,28 +2615,23 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2606,7 +2660,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>130</v>
       </c>
@@ -2626,7 +2680,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>222</v>
       </c>
@@ -2634,7 +2688,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>223</v>
       </c>
@@ -2642,7 +2696,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>136</v>
       </c>
@@ -2662,7 +2716,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>214</v>
       </c>
@@ -2670,7 +2724,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
         <v>216</v>
       </c>
@@ -2678,7 +2732,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>150</v>
       </c>
@@ -2698,7 +2752,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>226</v>
       </c>
@@ -2706,7 +2760,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>227</v>
       </c>
@@ -2714,7 +2768,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>230</v>
       </c>
@@ -2722,7 +2776,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>152</v>
       </c>
@@ -2742,7 +2796,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>218</v>
       </c>
@@ -2750,23 +2804,119 @@
         <v>219</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>220</v>
       </c>
       <c r="B22" t="s">
         <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>161</v>
+      </c>
+      <c r="D24" t="s">
+        <v>175</v>
+      </c>
+      <c r="E24">
+        <v>30</v>
+      </c>
+      <c r="F24">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>233</v>
+      </c>
+      <c r="B26" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B27" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>237</v>
+      </c>
+      <c r="B28" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>238</v>
+      </c>
+      <c r="B29" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" t="s">
+        <v>161</v>
+      </c>
+      <c r="D31" t="s">
+        <v>175</v>
+      </c>
+      <c r="E31">
+        <v>25</v>
+      </c>
+      <c r="F31">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>239</v>
+      </c>
+      <c r="B33" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>243</v>
+      </c>
+      <c r="B34" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>244</v>
+      </c>
+      <c r="B35" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="26" x14ac:dyDescent="0.15">
+      <c r="B36" s="16" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2778,9 +2928,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2812,11 +2962,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2828,9 +2973,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2862,11 +3007,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2874,17 +3014,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>114</v>
       </c>
@@ -2895,7 +3035,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
+    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -2906,7 +3046,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -2917,7 +3057,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -2928,7 +3068,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -2939,7 +3079,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -2950,7 +3090,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -2961,7 +3101,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45">
+    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -2972,7 +3112,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -2983,7 +3123,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -2994,7 +3134,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15">
+    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -3005,7 +3145,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15">
+    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -3016,7 +3156,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30">
+    <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -3027,7 +3167,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30">
+    <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -3038,7 +3178,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15">
+    <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -3049,7 +3189,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>129</v>
       </c>
@@ -3060,7 +3200,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15">
+    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>130</v>
       </c>
@@ -3071,7 +3211,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>131</v>
       </c>
@@ -3082,7 +3222,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>132</v>
       </c>
@@ -3093,7 +3233,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -3104,7 +3244,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15">
+    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>134</v>
       </c>
@@ -3115,7 +3255,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30">
+    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>135</v>
       </c>
@@ -3126,7 +3266,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30">
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>136</v>
       </c>
@@ -3137,7 +3277,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30">
+    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>137</v>
       </c>
@@ -3148,7 +3288,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30">
+    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>138</v>
       </c>
@@ -3159,7 +3299,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30">
+    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>139</v>
       </c>
@@ -3170,7 +3310,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="60">
+    <row r="27" spans="1:3" ht="80" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>140</v>
       </c>
@@ -3181,7 +3321,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>141</v>
       </c>
@@ -3192,7 +3332,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15">
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>142</v>
       </c>
@@ -3203,7 +3343,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -3214,7 +3354,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>144</v>
       </c>
@@ -3225,7 +3365,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30">
+    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -3236,7 +3376,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>146</v>
       </c>
@@ -3247,7 +3387,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30">
+    <row r="34" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>147</v>
       </c>
@@ -3258,7 +3398,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30">
+    <row r="35" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>148</v>
       </c>
@@ -3269,7 +3409,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30">
+    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>149</v>
       </c>
@@ -3280,7 +3420,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15">
+    <row r="37" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>150</v>
       </c>
@@ -3291,7 +3431,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30">
+    <row r="38" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -3302,7 +3442,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30">
+    <row r="39" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>152</v>
       </c>
@@ -3313,7 +3453,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30">
+    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>153</v>
       </c>
@@ -3324,7 +3464,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30">
+    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>154</v>
       </c>
@@ -3335,7 +3475,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15">
+    <row r="42" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>155</v>
       </c>
@@ -3346,7 +3486,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30">
+    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>156</v>
       </c>
@@ -3360,10 +3500,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Choosing user stories for sprint 4
</commit_message>
<xml_diff>
--- a/Team Report_Rafif, Maha, Saloni-Final.xlsx
+++ b/Team Report_Rafif, Maha, Saloni-Final.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="272">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -854,6 +854,30 @@
   </si>
   <si>
     <t>count should be less than 15</t>
+  </si>
+  <si>
+    <t>T28.01</t>
+  </si>
+  <si>
+    <t>T28.02</t>
+  </si>
+  <si>
+    <t>T28.03</t>
+  </si>
+  <si>
+    <t>Find children in the family</t>
+  </si>
+  <si>
+    <t>List in order of their birth</t>
+  </si>
+  <si>
+    <t>T30.01</t>
+  </si>
+  <si>
+    <t>T30.02</t>
+  </si>
+  <si>
+    <t>Check if they're living or dead</t>
   </si>
 </sst>
 </file>
@@ -3126,7 +3150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
@@ -3266,13 +3290,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
@@ -3301,6 +3328,80 @@
       </c>
       <c r="I1" s="9" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>270</v>
+      </c>
+      <c r="B11" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -3313,8 +3414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A27" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3677,6 +3778,9 @@
       <c r="C29" s="11" t="s">
         <v>51</v>
       </c>
+      <c r="D29" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
@@ -3701,6 +3805,9 @@
       </c>
       <c r="C31" s="11" t="s">
         <v>53</v>
+      </c>
+      <c r="D31" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
chose US for sprint 3
</commit_message>
<xml_diff>
--- a/Team Report_Rafif, Maha, Saloni-Final.xlsx
+++ b/Team Report_Rafif, Maha, Saloni-Final.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26207"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salonisetia/Documents/SSW-555-GEDCOM/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2460" yWindow="40" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId7"/>
     <sheet name="Stories" sheetId="11" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="283">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -878,6 +873,39 @@
   </si>
   <si>
     <t>Check if they're living or dead</t>
+  </si>
+  <si>
+    <t>find birthdate</t>
+  </si>
+  <si>
+    <t>compare birth date to today</t>
+  </si>
+  <si>
+    <t>T35.01</t>
+  </si>
+  <si>
+    <t>T35.02</t>
+  </si>
+  <si>
+    <t>T35.03</t>
+  </si>
+  <si>
+    <t>Find Marriage date for each family</t>
+  </si>
+  <si>
+    <t>compare to today</t>
+  </si>
+  <si>
+    <t>print marriage date for next month</t>
+  </si>
+  <si>
+    <t>T39.01</t>
+  </si>
+  <si>
+    <t>T39.02</t>
+  </si>
+  <si>
+    <t>T39.03</t>
   </si>
 </sst>
 </file>
@@ -936,7 +964,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -993,6 +1021,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1049,7 +1093,7 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1098,6 +1142,22 @@
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1209,11 +1269,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2140054496"/>
-        <c:axId val="-2139275904"/>
+        <c:axId val="-2145426552"/>
+        <c:axId val="2074522616"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2140054496"/>
+        <c:axId val="-2145426552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1223,14 +1283,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139275904"/>
+        <c:crossAx val="2074522616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2139275904"/>
+        <c:axId val="2074522616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1241,7 +1301,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140054496"/>
+        <c:crossAx val="-2145426552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1619,15 +1679,15 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -1644,7 +1704,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>159</v>
       </c>
@@ -1661,7 +1721,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>160</v>
       </c>
@@ -1678,7 +1738,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -1695,7 +1755,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="D9" s="4" t="s">
         <v>29</v>
       </c>
@@ -1715,6 +1775,11 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1722,20 +1787,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>209</v>
       </c>
@@ -1752,7 +1817,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1769,7 +1834,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1786,7 +1851,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1803,7 +1868,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="B5" t="s">
         <v>118</v>
       </c>
@@ -1811,7 +1876,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1828,7 +1893,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="B7" t="s">
         <v>120</v>
       </c>
@@ -1836,7 +1901,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1853,7 +1918,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="B9" t="s">
         <v>122</v>
       </c>
@@ -1861,7 +1926,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="B10" t="s">
         <v>123</v>
       </c>
@@ -1869,7 +1934,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1886,7 +1951,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5">
       <c r="B12" t="s">
         <v>125</v>
       </c>
@@ -1894,7 +1959,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5">
       <c r="B13" t="s">
         <v>126</v>
       </c>
@@ -1902,7 +1967,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5">
       <c r="B14" t="s">
         <v>127</v>
       </c>
@@ -1910,7 +1975,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5">
       <c r="B15" t="s">
         <v>128</v>
       </c>
@@ -1918,7 +1983,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1935,7 +2000,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1952,7 +2017,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5">
       <c r="B18" t="s">
         <v>131</v>
       </c>
@@ -1960,7 +2025,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5">
       <c r="B19" t="s">
         <v>132</v>
       </c>
@@ -1968,7 +2033,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5">
       <c r="B20" t="s">
         <v>133</v>
       </c>
@@ -1976,7 +2041,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5">
       <c r="B21" t="s">
         <v>134</v>
       </c>
@@ -1984,7 +2049,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5">
       <c r="B22" t="s">
         <v>135</v>
       </c>
@@ -1992,7 +2057,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2009,7 +2074,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2026,7 +2091,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5">
       <c r="B25" t="s">
         <v>138</v>
       </c>
@@ -2034,7 +2099,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5">
       <c r="B26" t="s">
         <v>139</v>
       </c>
@@ -2042,7 +2107,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5">
       <c r="B27" t="s">
         <v>140</v>
       </c>
@@ -2050,7 +2115,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2067,7 +2132,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5">
       <c r="B29" t="s">
         <v>142</v>
       </c>
@@ -2075,7 +2140,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2092,7 +2157,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5">
       <c r="B31" t="s">
         <v>144</v>
       </c>
@@ -2100,7 +2165,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>3</v>
+      </c>
       <c r="B32" t="s">
         <v>145</v>
       </c>
@@ -2108,7 +2176,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5">
       <c r="B33" t="s">
         <v>146</v>
       </c>
@@ -2116,7 +2184,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5">
       <c r="B34" t="s">
         <v>147</v>
       </c>
@@ -2124,7 +2192,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5">
       <c r="B35" t="s">
         <v>148</v>
       </c>
@@ -2132,15 +2200,24 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>3</v>
+      </c>
       <c r="B36" t="s">
         <v>149</v>
       </c>
       <c r="C36" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D36" t="s">
+        <v>160</v>
+      </c>
+      <c r="E36" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>2</v>
       </c>
@@ -2157,7 +2234,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5">
       <c r="B38" t="s">
         <v>151</v>
       </c>
@@ -2165,7 +2242,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>2</v>
       </c>
@@ -2182,15 +2259,24 @@
         <v>212</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>3</v>
+      </c>
       <c r="B40" t="s">
         <v>153</v>
       </c>
       <c r="C40" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D40" t="s">
+        <v>160</v>
+      </c>
+      <c r="E40" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="B41" t="s">
         <v>154</v>
       </c>
@@ -2198,7 +2284,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5">
       <c r="B42" t="s">
         <v>155</v>
       </c>
@@ -2206,7 +2292,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5">
       <c r="B43" t="s">
         <v>156</v>
       </c>
@@ -2218,6 +2304,11 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2229,17 +2320,17 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="2"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2259,7 +2350,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>40440</v>
       </c>
@@ -2279,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>40454</v>
       </c>
@@ -2301,7 +2392,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>41193</v>
       </c>
@@ -2328,6 +2419,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2339,21 +2435,21 @@
       <selection activeCell="B37" sqref="B37:B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="6"/>
-    <col min="11" max="11" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="6"/>
+    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2382,7 +2478,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
         <v>115</v>
       </c>
@@ -2411,10 +2507,10 @@
         <v>41182</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9">
       <c r="A4" s="14" t="s">
         <v>183</v>
       </c>
@@ -2422,7 +2518,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="A5" s="14" t="s">
         <v>184</v>
       </c>
@@ -2430,10 +2526,10 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9">
       <c r="A6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
         <v>117</v>
       </c>
@@ -2462,10 +2558,10 @@
         <v>41184</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>177</v>
       </c>
@@ -2473,7 +2569,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>179</v>
       </c>
@@ -2481,7 +2577,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>181</v>
       </c>
@@ -2489,7 +2585,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9">
       <c r="A13" s="4" t="s">
         <v>121</v>
       </c>
@@ -2518,11 +2614,11 @@
         <v>41181</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9">
       <c r="A14" s="4"/>
       <c r="B14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="A15" s="14" t="s">
         <v>187</v>
       </c>
@@ -2530,7 +2626,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9">
       <c r="A16" s="14" t="s">
         <v>188</v>
       </c>
@@ -2538,7 +2634,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="39" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" ht="26">
       <c r="A17" s="14" t="s">
         <v>199</v>
       </c>
@@ -2546,7 +2642,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="39" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="26">
       <c r="A18" s="14" t="s">
         <v>200</v>
       </c>
@@ -2554,10 +2650,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9">
       <c r="A20" s="4" t="s">
         <v>137</v>
       </c>
@@ -2586,11 +2682,11 @@
         <v>41184</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9">
       <c r="A21" s="4"/>
       <c r="B21"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9">
       <c r="A22" s="14" t="s">
         <v>194</v>
       </c>
@@ -2598,7 +2694,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9">
       <c r="A23" s="14" t="s">
         <v>195</v>
       </c>
@@ -2606,7 +2702,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="26">
       <c r="A24" s="14" t="s">
         <v>196</v>
       </c>
@@ -2614,11 +2710,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9">
       <c r="A26" s="4" t="s">
         <v>141</v>
       </c>
@@ -2647,11 +2743,11 @@
         <v>41184</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9">
       <c r="A27" s="4"/>
       <c r="B27"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9">
       <c r="A28" s="14" t="s">
         <v>190</v>
       </c>
@@ -2659,11 +2755,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9">
       <c r="A29" s="14"/>
       <c r="B29"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9">
       <c r="A30" s="4" t="s">
         <v>143</v>
       </c>
@@ -2692,11 +2788,11 @@
         <v>41184</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9">
       <c r="A31" s="4"/>
       <c r="B31"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9">
       <c r="A32" s="14" t="s">
         <v>203</v>
       </c>
@@ -2704,7 +2800,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2">
       <c r="A33" s="14" t="s">
         <v>206</v>
       </c>
@@ -2712,35 +2808,35 @@
         <v>205</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2">
       <c r="B35" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2">
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2">
       <c r="B37" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2">
       <c r="B38" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2">
       <c r="B39" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2">
       <c r="B41" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2">
       <c r="B42" s="1" t="s">
         <v>231</v>
       </c>
@@ -2749,6 +2845,11 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2756,16 +2857,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A5" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2794,7 +2895,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
         <v>130</v>
       </c>
@@ -2823,7 +2924,7 @@
         <v>41192</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9">
       <c r="A4" s="14" t="s">
         <v>221</v>
       </c>
@@ -2831,7 +2932,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="A5" s="14" t="s">
         <v>222</v>
       </c>
@@ -2839,7 +2940,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
         <v>136</v>
       </c>
@@ -2868,7 +2969,7 @@
         <v>41192</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9">
       <c r="A9" s="14" t="s">
         <v>213</v>
       </c>
@@ -2876,7 +2977,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="A10" s="14" t="s">
         <v>215</v>
       </c>
@@ -2884,7 +2985,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9">
       <c r="A13" s="4" t="s">
         <v>150</v>
       </c>
@@ -2913,7 +3014,7 @@
         <v>41193</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>225</v>
       </c>
@@ -2921,7 +3022,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>226</v>
       </c>
@@ -2929,7 +3030,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>229</v>
       </c>
@@ -2937,7 +3038,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9">
       <c r="A19" s="4" t="s">
         <v>152</v>
       </c>
@@ -2966,7 +3067,7 @@
         <v>41193</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>217</v>
       </c>
@@ -2974,7 +3075,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>219</v>
       </c>
@@ -2982,7 +3083,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9">
       <c r="A24" s="4" t="s">
         <v>116</v>
       </c>
@@ -3011,7 +3112,7 @@
         <v>41193</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>232</v>
       </c>
@@ -3019,7 +3120,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>235</v>
       </c>
@@ -3027,7 +3128,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>236</v>
       </c>
@@ -3035,7 +3136,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>237</v>
       </c>
@@ -3043,7 +3144,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9">
       <c r="A31" s="4" t="s">
         <v>124</v>
       </c>
@@ -3072,7 +3173,7 @@
         <v>41193</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>238</v>
       </c>
@@ -3080,7 +3181,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>242</v>
       </c>
@@ -3088,7 +3189,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>243</v>
       </c>
@@ -3096,7 +3197,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2" ht="26">
       <c r="A36" t="s">
         <v>244</v>
       </c>
@@ -3104,55 +3205,55 @@
         <v>240</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2">
       <c r="B38" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2">
       <c r="B40" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2">
       <c r="B41" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2">
       <c r="B42" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2">
       <c r="B43" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2" ht="26">
       <c r="B44" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2">
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2">
       <c r="B46" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2">
       <c r="B47" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2">
       <c r="B48" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:2">
       <c r="B49" s="1" t="s">
         <v>249</v>
       </c>
@@ -3161,23 +3262,28 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="39.33203125" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3206,7 +3312,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
         <v>119</v>
       </c>
@@ -3226,10 +3332,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9">
       <c r="A4" s="14" t="s">
         <v>253</v>
       </c>
@@ -3237,7 +3343,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="A5" s="14" t="s">
         <v>254</v>
       </c>
@@ -3245,7 +3351,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9">
       <c r="A6" s="14" t="s">
         <v>255</v>
       </c>
@@ -3253,7 +3359,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9">
       <c r="A7" s="14" t="s">
         <v>259</v>
       </c>
@@ -3261,10 +3367,10 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9">
       <c r="A8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
         <v>129</v>
       </c>
@@ -3284,7 +3390,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>260</v>
       </c>
@@ -3292,17 +3398,111 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>261</v>
       </c>
       <c r="B12" t="s">
         <v>263</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14" t="s">
+        <v>252</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+      <c r="F14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>274</v>
+      </c>
+      <c r="B16" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>275</v>
+      </c>
+      <c r="B17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>276</v>
+      </c>
+      <c r="B18" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" t="s">
+        <v>252</v>
+      </c>
+      <c r="E21">
+        <v>35</v>
+      </c>
+      <c r="F21">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>280</v>
+      </c>
+      <c r="B23" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>281</v>
+      </c>
+      <c r="B24" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>282</v>
+      </c>
+      <c r="B25" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3314,12 +3514,12 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3348,7 +3548,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
         <v>142</v>
       </c>
@@ -3365,7 +3565,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>264</v>
       </c>
@@ -3373,7 +3573,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>265</v>
       </c>
@@ -3381,7 +3581,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>266</v>
       </c>
@@ -3389,7 +3589,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
         <v>144</v>
       </c>
@@ -3406,7 +3606,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>269</v>
       </c>
@@ -3414,7 +3614,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>270</v>
       </c>
@@ -3425,6 +3625,11 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3436,13 +3641,13 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>114</v>
       </c>
@@ -3456,7 +3661,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="30">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -3470,7 +3675,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -3484,7 +3689,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -3498,7 +3703,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -3509,7 +3714,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -3523,7 +3728,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="15">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -3534,7 +3739,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="45">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -3548,7 +3753,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="30">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -3559,7 +3764,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="30">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -3570,7 +3775,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -3584,7 +3789,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="15">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -3595,7 +3800,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="48" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -3606,7 +3811,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="30">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -3617,7 +3822,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="15">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -3628,7 +3833,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="15">
       <c r="A16" t="s">
         <v>129</v>
       </c>
@@ -3642,7 +3847,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="15">
       <c r="A17" t="s">
         <v>130</v>
       </c>
@@ -3656,7 +3861,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15">
       <c r="A18" t="s">
         <v>131</v>
       </c>
@@ -3667,7 +3872,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15">
       <c r="A19" t="s">
         <v>132</v>
       </c>
@@ -3678,7 +3883,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -3689,7 +3894,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="15">
       <c r="A21" t="s">
         <v>134</v>
       </c>
@@ -3700,7 +3905,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="30">
       <c r="A22" t="s">
         <v>135</v>
       </c>
@@ -3711,7 +3916,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="30">
       <c r="A23" t="s">
         <v>136</v>
       </c>
@@ -3725,7 +3930,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="30">
       <c r="A24" t="s">
         <v>137</v>
       </c>
@@ -3739,7 +3944,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="48" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="30">
       <c r="A25" t="s">
         <v>138</v>
       </c>
@@ -3750,7 +3955,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="30">
       <c r="A26" t="s">
         <v>139</v>
       </c>
@@ -3761,7 +3966,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="80" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="60">
       <c r="A27" t="s">
         <v>140</v>
       </c>
@@ -3772,7 +3977,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15">
       <c r="A28" t="s">
         <v>141</v>
       </c>
@@ -3786,7 +3991,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="15">
       <c r="A29" t="s">
         <v>142</v>
       </c>
@@ -3800,7 +4005,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="15">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -3814,7 +4019,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="15">
       <c r="A31" t="s">
         <v>144</v>
       </c>
@@ -3828,7 +4033,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="30">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -3839,7 +4044,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="15">
       <c r="A33" t="s">
         <v>146</v>
       </c>
@@ -3850,7 +4055,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="30">
       <c r="A34" t="s">
         <v>147</v>
       </c>
@@ -3861,7 +4066,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="48" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="30">
       <c r="A35" t="s">
         <v>148</v>
       </c>
@@ -3872,7 +4077,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="30">
       <c r="A36" t="s">
         <v>149</v>
       </c>
@@ -3883,7 +4088,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="15">
       <c r="A37" t="s">
         <v>150</v>
       </c>
@@ -3897,7 +4102,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="30">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -3908,7 +4113,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="30">
       <c r="A39" t="s">
         <v>152</v>
       </c>
@@ -3922,7 +4127,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="30">
       <c r="A40" t="s">
         <v>153</v>
       </c>
@@ -3933,7 +4138,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="30">
       <c r="A41" t="s">
         <v>154</v>
       </c>
@@ -3944,7 +4149,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="15">
       <c r="A42" t="s">
         <v>155</v>
       </c>
@@ -3955,7 +4160,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="30">
       <c r="A43" t="s">
         <v>156</v>
       </c>
@@ -3969,5 +4174,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update sprint 3 user story
</commit_message>
<xml_diff>
--- a/Team Report_Rafif, Maha, Saloni-Final.xlsx
+++ b/Team Report_Rafif, Maha, Saloni-Final.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="291">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -916,24 +916,6 @@
     <t>T39.03</t>
   </si>
   <si>
-    <t>T25.01</t>
-  </si>
-  <si>
-    <t>find first name for individual</t>
-  </si>
-  <si>
-    <t>T25.02</t>
-  </si>
-  <si>
-    <t>check same family</t>
-  </si>
-  <si>
-    <t>T25.03</t>
-  </si>
-  <si>
-    <t>check unique first name</t>
-  </si>
-  <si>
     <t>T21.01</t>
   </si>
   <si>
@@ -944,6 +926,18 @@
   </si>
   <si>
     <t>check correct gender</t>
+  </si>
+  <si>
+    <t>T31.01</t>
+  </si>
+  <si>
+    <t>T31.02</t>
+  </si>
+  <si>
+    <t>Check age over 30</t>
+  </si>
+  <si>
+    <t>check single people</t>
   </si>
 </sst>
 </file>
@@ -1307,11 +1301,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="735540208"/>
-        <c:axId val="768527840"/>
+        <c:axId val="788299120"/>
+        <c:axId val="764528144"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="735540208"/>
+        <c:axId val="788299120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1321,14 +1315,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="768527840"/>
+        <c:crossAx val="764528144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="768527840"/>
+        <c:axId val="764528144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,7 +1333,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="735540208"/>
+        <c:crossAx val="788299120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3306,7 +3300,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3465,26 +3459,26 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B15" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B16" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C18" t="s">
         <v>162</v>
@@ -3493,7 +3487,7 @@
         <v>252</v>
       </c>
       <c r="E18">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F18">
         <v>60</v>
@@ -3501,26 +3495,18 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="B19" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B20" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>287</v>
-      </c>
-      <c r="B21" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
@@ -3745,7 +3731,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView topLeftCell="A27" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B32" sqref="A32:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Update sprint 4 user stories
</commit_message>
<xml_diff>
--- a/Team Report_Rafif, Maha, Saloni-Final.xlsx
+++ b/Team Report_Rafif, Maha, Saloni-Final.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="304">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -938,6 +938,45 @@
   </si>
   <si>
     <t>check single people</t>
+  </si>
+  <si>
+    <t>T04.01</t>
+  </si>
+  <si>
+    <t>Find mariage date</t>
+  </si>
+  <si>
+    <t>Find divorce date</t>
+  </si>
+  <si>
+    <t>Check if divorce happens before marriage</t>
+  </si>
+  <si>
+    <t>T04.02</t>
+  </si>
+  <si>
+    <t>T04.03</t>
+  </si>
+  <si>
+    <t>T06.01</t>
+  </si>
+  <si>
+    <t>Find their divorce date</t>
+  </si>
+  <si>
+    <t>Find death date</t>
+  </si>
+  <si>
+    <t>Check if death happens before divorce</t>
+  </si>
+  <si>
+    <t>T06.02</t>
+  </si>
+  <si>
+    <t>T06.03</t>
+  </si>
+  <si>
+    <t>T06.04</t>
   </si>
 </sst>
 </file>
@@ -1301,11 +1340,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="781867632"/>
-        <c:axId val="781774384"/>
+        <c:axId val="780217152"/>
+        <c:axId val="784938816"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="781867632"/>
+        <c:axId val="780217152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1315,14 +1354,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="781774384"/>
+        <c:crossAx val="784938816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="781774384"/>
+        <c:axId val="784938816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,7 +1372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="781867632"/>
+        <c:crossAx val="780217152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1814,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32:E32"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1896,11 +1935,20 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>118</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -1921,11 +1969,20 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>4</v>
+      </c>
       <c r="B7" t="s">
         <v>120</v>
       </c>
       <c r="C7" t="s">
         <v>71</v>
+      </c>
+      <c r="D7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -2463,7 +2520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B37" sqref="B37:B42"/>
     </sheetView>
   </sheetViews>
@@ -2884,8 +2941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:B22"/>
+    <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3603,15 +3660,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
@@ -3715,6 +3772,102 @@
       </c>
       <c r="B11" t="s">
         <v>271</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" t="s">
+        <v>252</v>
+      </c>
+      <c r="E13">
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>295</v>
+      </c>
+      <c r="B15" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>296</v>
+      </c>
+      <c r="B16" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D18" t="s">
+        <v>252</v>
+      </c>
+      <c r="E18">
+        <v>30</v>
+      </c>
+      <c r="F18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>297</v>
+      </c>
+      <c r="B19" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>301</v>
+      </c>
+      <c r="B20" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>302</v>
+      </c>
+      <c r="B21" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>303</v>
+      </c>
+      <c r="B22" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -3727,8 +3880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B32" sqref="A32:B32"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Update Sprint 3 user stories and report
</commit_message>
<xml_diff>
--- a/Team Report_Rafif, Maha, Saloni-Final.xlsx
+++ b/Team Report_Rafif, Maha, Saloni-Final.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27610"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2460" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -1340,11 +1340,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="780217152"/>
-        <c:axId val="784938816"/>
+        <c:axId val="1306140048"/>
+        <c:axId val="1306142368"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="780217152"/>
+        <c:axId val="1306140048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1354,14 +1354,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="784938816"/>
+        <c:crossAx val="1306142368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="784938816"/>
+        <c:axId val="1306142368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1372,7 +1372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="780217152"/>
+        <c:crossAx val="1306140048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1853,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2147,7 +2147,7 @@
         <v>159</v>
       </c>
       <c r="E22" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
@@ -2272,7 +2272,7 @@
         <v>159</v>
       </c>
       <c r="E32" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
@@ -3353,8 +3353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3499,16 +3499,25 @@
         <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D14" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="E14">
         <v>35</v>
       </c>
       <c r="F14">
         <v>60</v>
+      </c>
+      <c r="G14">
+        <v>39</v>
+      </c>
+      <c r="H14">
+        <v>20</v>
+      </c>
+      <c r="I14" s="17">
+        <v>41203</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
@@ -3527,7 +3536,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>145</v>
       </c>
@@ -3535,10 +3544,10 @@
         <v>101</v>
       </c>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D18" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="E18">
         <v>30</v>
@@ -3546,8 +3555,17 @@
       <c r="F18">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G18">
+        <v>25</v>
+      </c>
+      <c r="H18">
+        <v>15</v>
+      </c>
+      <c r="I18" s="17">
+        <v>41203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>287</v>
       </c>
@@ -3555,7 +3573,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>288</v>
       </c>
@@ -3563,7 +3581,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>149</v>
       </c>
@@ -3583,7 +3601,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>274</v>
       </c>
@@ -3591,7 +3609,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>275</v>
       </c>
@@ -3599,7 +3617,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>276</v>
       </c>
@@ -3607,7 +3625,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>153</v>
       </c>
@@ -3627,7 +3645,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>280</v>
       </c>

</xml_diff>

<commit_message>
Updated sprint 3 sheet
</commit_message>
<xml_diff>
--- a/Team Report_Rafif, Maha, Saloni-Final.xlsx
+++ b/Team Report_Rafif, Maha, Saloni-Final.xlsx
@@ -1030,7 +1030,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="98">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1087,6 +1087,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1164,7 +1165,7 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="98">
+  <cellStyles count="99">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1234,6 +1235,7 @@
     <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1345,11 +1347,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132053560"/>
-        <c:axId val="2132056680"/>
+        <c:axId val="2139896072"/>
+        <c:axId val="2139899144"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2132053560"/>
+        <c:axId val="2139896072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1359,14 +1361,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132056680"/>
+        <c:crossAx val="2139899144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2132056680"/>
+        <c:axId val="2139899144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1377,7 +1379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132053560"/>
+        <c:crossAx val="2139896072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3398,8 +3400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3672,13 +3674,22 @@
         <v>165</v>
       </c>
       <c r="D30" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="E30">
         <v>35</v>
       </c>
       <c r="F30">
         <v>60</v>
+      </c>
+      <c r="G30">
+        <v>23</v>
+      </c>
+      <c r="H30">
+        <v>24</v>
+      </c>
+      <c r="I30" s="17">
+        <v>41203</v>
       </c>
     </row>
     <row r="32" spans="1:9">

</xml_diff>

<commit_message>
fixed bugs in US39
</commit_message>
<xml_diff>
--- a/Team Report_Rafif, Maha, Saloni-Final.xlsx
+++ b/Team Report_Rafif, Maha, Saloni-Final.xlsx
@@ -1347,11 +1347,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2139896072"/>
-        <c:axId val="2139899144"/>
+        <c:axId val="2142105992"/>
+        <c:axId val="2142109064"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2139896072"/>
+        <c:axId val="2142105992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1361,14 +1361,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139899144"/>
+        <c:crossAx val="2142109064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2139899144"/>
+        <c:axId val="2142109064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1379,7 +1379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139896072"/>
+        <c:crossAx val="2142105992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3400,8 +3400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3683,10 +3683,10 @@
         <v>60</v>
       </c>
       <c r="G30">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H30">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="I30" s="17">
         <v>41203</v>

</xml_diff>

<commit_message>
Adding US28 - Sprint 4
</commit_message>
<xml_diff>
--- a/Team Report_Rafif, Maha, Saloni-Final.xlsx
+++ b/Team Report_Rafif, Maha, Saloni-Final.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="1260" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="3160" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="304">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1872,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2260,6 +2260,9 @@
       <c r="D29" t="s">
         <v>161</v>
       </c>
+      <c r="E29" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
@@ -2290,6 +2293,9 @@
       </c>
       <c r="D31" t="s">
         <v>161</v>
+      </c>
+      <c r="E31" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
@@ -3737,8 +3743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3786,13 +3792,22 @@
         <v>161</v>
       </c>
       <c r="D2" t="s">
-        <v>251</v>
+        <v>211</v>
       </c>
       <c r="E2">
         <v>30</v>
       </c>
       <c r="F2">
         <v>60</v>
+      </c>
+      <c r="G2">
+        <v>28</v>
+      </c>
+      <c r="H2">
+        <v>40</v>
+      </c>
+      <c r="I2" s="17">
+        <v>41207</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
added sprint 4 planning
</commit_message>
<xml_diff>
--- a/Team Report_Rafif, Maha, Saloni-Final.xlsx
+++ b/Team Report_Rafif, Maha, Saloni-Final.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="2460" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="316">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -972,6 +972,42 @@
   </si>
   <si>
     <t>malidrisi</t>
+  </si>
+  <si>
+    <t>T25.01</t>
+  </si>
+  <si>
+    <t>T25.02</t>
+  </si>
+  <si>
+    <t>T25.03</t>
+  </si>
+  <si>
+    <t>T25.04</t>
+  </si>
+  <si>
+    <t>define a list for each family names</t>
+  </si>
+  <si>
+    <t>add husband and wife names</t>
+  </si>
+  <si>
+    <t>add children names</t>
+  </si>
+  <si>
+    <t>check if sthe list has repeated name</t>
+  </si>
+  <si>
+    <t>T24.01</t>
+  </si>
+  <si>
+    <t>T24.02</t>
+  </si>
+  <si>
+    <t>T24.03</t>
+  </si>
+  <si>
+    <t>T24.04</t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1066,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1087,6 +1123,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1167,7 +1211,7 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="109">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1240,6 +1284,14 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1357,11 +1409,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2100141992"/>
-        <c:axId val="-2099895912"/>
+        <c:axId val="2131348200"/>
+        <c:axId val="-2103631960"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2100141992"/>
+        <c:axId val="2131348200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1371,14 +1423,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099895912"/>
+        <c:crossAx val="-2103631960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2099895912"/>
+        <c:axId val="-2103631960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,7 +1441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2100141992"/>
+        <c:crossAx val="2131348200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1875,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2207,11 +2259,17 @@
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="A25">
+        <v>4</v>
+      </c>
       <c r="B25" t="s">
         <v>138</v>
       </c>
       <c r="C25" t="s">
         <v>93</v>
+      </c>
+      <c r="D25" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2223,6 +2281,12 @@
       </c>
       <c r="C26" t="s">
         <v>94</v>
+      </c>
+      <c r="D26" t="s">
+        <v>160</v>
+      </c>
+      <c r="E26" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3004,7 +3068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="150" workbookViewId="0">
       <selection activeCell="H31" sqref="H2:H31"/>
     </sheetView>
   </sheetViews>
@@ -3421,7 +3485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="150" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -3751,10 +3815,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:B24"/>
+    <sheetView topLeftCell="A11" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3962,16 +4026,113 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" t="s">
+      <c r="A24" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" t="s">
+        <v>160</v>
+      </c>
+      <c r="D24" t="s">
+        <v>251</v>
+      </c>
+      <c r="E24">
+        <v>35</v>
+      </c>
+      <c r="F24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>312</v>
+      </c>
+      <c r="B26" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>313</v>
+      </c>
+      <c r="B27" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>314</v>
+      </c>
+      <c r="B28" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>315</v>
+      </c>
+      <c r="B29" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B33" s="4" t="s">
         <v>94</v>
+      </c>
+      <c r="C33" t="s">
+        <v>160</v>
+      </c>
+      <c r="D33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E33">
+        <v>35</v>
+      </c>
+      <c r="F33">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>304</v>
+      </c>
+      <c r="B35" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>305</v>
+      </c>
+      <c r="B36" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>306</v>
+      </c>
+      <c r="B37" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>307</v>
+      </c>
+      <c r="B38" t="s">
+        <v>311</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3984,8 +4145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
report re-updated sprint 4
</commit_message>
<xml_diff>
--- a/Team Report_Rafif, Maha, Saloni-Final.xlsx
+++ b/Team Report_Rafif, Maha, Saloni-Final.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="980" yWindow="520" windowWidth="27820" windowHeight="16860" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="980" yWindow="520" windowWidth="27820" windowHeight="16860" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -1427,11 +1427,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2039050096"/>
-        <c:axId val="-2039393888"/>
+        <c:axId val="-2003809120"/>
+        <c:axId val="-2003327232"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2039050096"/>
+        <c:axId val="-2003809120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1441,14 +1441,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2039393888"/>
+        <c:crossAx val="-2003327232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2039393888"/>
+        <c:axId val="-2003327232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1459,7 +1459,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2039050096"/>
+        <c:crossAx val="-2003809120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2664,7 +2664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="H30" sqref="H2:H30"/>
     </sheetView>
   </sheetViews>
@@ -3085,7 +3085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B38" sqref="B38:B49"/>
     </sheetView>
   </sheetViews>
@@ -3497,7 +3497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -3912,8 +3912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4065,7 +4065,7 @@
         <v>30</v>
       </c>
       <c r="F13">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
@@ -4109,7 +4109,7 @@
         <v>30</v>
       </c>
       <c r="F18">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
added US24 and US25
</commit_message>
<xml_diff>
--- a/Team Report_Rafif, Maha, Saloni-Final.xlsx
+++ b/Team Report_Rafif, Maha, Saloni-Final.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafifarab/Desktop/SSW-555-GEDCOM/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="980" yWindow="520" windowWidth="27820" windowHeight="16860" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -21,13 +16,13 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId7"/>
     <sheet name="Stories" sheetId="11" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -1080,7 +1075,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="111">
+  <cellStyleXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1137,6 +1132,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1227,7 +1228,7 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="111">
+  <cellStyles count="117">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1310,6 +1311,12 @@
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1427,11 +1434,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2002756944"/>
-        <c:axId val="-2046661040"/>
+        <c:axId val="-2096541624"/>
+        <c:axId val="-2096624280"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2002756944"/>
+        <c:axId val="-2096541624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1441,14 +1448,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2046661040"/>
+        <c:crossAx val="-2096624280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2046661040"/>
+        <c:axId val="-2096624280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1459,7 +1466,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2002756944"/>
+        <c:crossAx val="-2096541624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1837,15 +1844,15 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -1862,7 +1869,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>159</v>
       </c>
@@ -1879,7 +1886,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>160</v>
       </c>
@@ -1896,7 +1903,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -1913,7 +1920,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="D9" s="4" t="s">
         <v>29</v>
       </c>
@@ -1933,6 +1940,11 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1940,20 +1952,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>208</v>
       </c>
@@ -1970,7 +1982,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1987,7 +1999,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2004,7 +2016,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2021,7 +2033,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2038,7 +2050,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2055,7 +2067,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2072,7 +2084,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2089,7 +2101,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="B9" t="s">
         <v>122</v>
       </c>
@@ -2097,7 +2109,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="B10" t="s">
         <v>123</v>
       </c>
@@ -2105,7 +2117,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2122,7 +2134,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5">
       <c r="B12" t="s">
         <v>125</v>
       </c>
@@ -2130,7 +2142,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5">
       <c r="B13" t="s">
         <v>126</v>
       </c>
@@ -2138,7 +2150,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5">
       <c r="B14" t="s">
         <v>127</v>
       </c>
@@ -2146,7 +2158,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5">
       <c r="B15" t="s">
         <v>128</v>
       </c>
@@ -2154,7 +2166,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2171,7 +2183,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2188,7 +2200,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5">
       <c r="B18" t="s">
         <v>131</v>
       </c>
@@ -2196,7 +2208,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5">
       <c r="B19" t="s">
         <v>132</v>
       </c>
@@ -2204,7 +2216,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5">
       <c r="B20" t="s">
         <v>133</v>
       </c>
@@ -2212,7 +2224,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5">
       <c r="B21" t="s">
         <v>134</v>
       </c>
@@ -2220,7 +2232,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2237,7 +2249,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2254,7 +2266,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2271,7 +2283,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>4</v>
       </c>
@@ -2285,10 +2297,10 @@
         <v>160</v>
       </c>
       <c r="E25" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>4</v>
       </c>
@@ -2302,10 +2314,10 @@
         <v>160</v>
       </c>
       <c r="E26" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="B27" t="s">
         <v>140</v>
       </c>
@@ -2313,7 +2325,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2330,7 +2342,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>4</v>
       </c>
@@ -2347,7 +2359,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2364,7 +2376,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2381,7 +2393,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2398,7 +2410,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5">
       <c r="B33" t="s">
         <v>146</v>
       </c>
@@ -2406,7 +2418,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5">
       <c r="B34" t="s">
         <v>147</v>
       </c>
@@ -2414,7 +2426,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5">
       <c r="B35" t="s">
         <v>148</v>
       </c>
@@ -2422,7 +2434,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2439,7 +2451,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>2</v>
       </c>
@@ -2456,7 +2468,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5">
       <c r="B38" t="s">
         <v>151</v>
       </c>
@@ -2464,7 +2476,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>2</v>
       </c>
@@ -2481,7 +2493,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2498,7 +2510,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5">
       <c r="B41" t="s">
         <v>154</v>
       </c>
@@ -2506,7 +2518,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5">
       <c r="B42" t="s">
         <v>155</v>
       </c>
@@ -2514,7 +2526,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5">
       <c r="B43" t="s">
         <v>156</v>
       </c>
@@ -2526,6 +2538,11 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2537,17 +2554,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="2"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2567,7 +2584,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>41171</v>
       </c>
@@ -2587,7 +2604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>41185</v>
       </c>
@@ -2609,7 +2626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>41193</v>
       </c>
@@ -2631,7 +2648,7 @@
         <v>9.5192307692307683</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6">
       <c r="A5" s="6">
         <v>41213</v>
       </c>
@@ -2657,6 +2674,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2668,21 +2690,21 @@
       <selection activeCell="H30" sqref="H2:H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="6"/>
-    <col min="11" max="11" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="6"/>
+    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2711,7 +2733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
         <v>115</v>
       </c>
@@ -2740,10 +2762,10 @@
         <v>41182</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9">
       <c r="A4" s="14" t="s">
         <v>182</v>
       </c>
@@ -2751,7 +2773,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="A5" s="14" t="s">
         <v>183</v>
       </c>
@@ -2759,10 +2781,10 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9">
       <c r="A6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
         <v>117</v>
       </c>
@@ -2791,10 +2813,10 @@
         <v>41184</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>176</v>
       </c>
@@ -2802,7 +2824,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -2810,7 +2832,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>180</v>
       </c>
@@ -2818,7 +2840,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9">
       <c r="A13" s="4" t="s">
         <v>121</v>
       </c>
@@ -2847,11 +2869,11 @@
         <v>41181</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9">
       <c r="A14" s="4"/>
       <c r="B14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="A15" s="14" t="s">
         <v>186</v>
       </c>
@@ -2859,7 +2881,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9">
       <c r="A16" s="14" t="s">
         <v>187</v>
       </c>
@@ -2867,7 +2889,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="39" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" ht="26">
       <c r="A17" s="14" t="s">
         <v>198</v>
       </c>
@@ -2875,7 +2897,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="39" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="26">
       <c r="A18" s="14" t="s">
         <v>199</v>
       </c>
@@ -2883,10 +2905,10 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9">
       <c r="A20" s="4" t="s">
         <v>137</v>
       </c>
@@ -2915,11 +2937,11 @@
         <v>41184</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9">
       <c r="A21" s="4"/>
       <c r="B21"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9">
       <c r="A22" s="14" t="s">
         <v>193</v>
       </c>
@@ -2927,7 +2949,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9">
       <c r="A23" s="14" t="s">
         <v>194</v>
       </c>
@@ -2935,7 +2957,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="26">
       <c r="A24" s="14" t="s">
         <v>195</v>
       </c>
@@ -2943,11 +2965,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9">
       <c r="A26" s="4" t="s">
         <v>141</v>
       </c>
@@ -2976,11 +2998,11 @@
         <v>41184</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9">
       <c r="A27" s="4"/>
       <c r="B27"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9">
       <c r="A28" s="14" t="s">
         <v>189</v>
       </c>
@@ -2988,11 +3010,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9">
       <c r="A29" s="14"/>
       <c r="B29"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9">
       <c r="A30" s="4" t="s">
         <v>143</v>
       </c>
@@ -3021,11 +3043,11 @@
         <v>41184</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9">
       <c r="A31" s="4"/>
       <c r="B31"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9">
       <c r="A32" s="14" t="s">
         <v>202</v>
       </c>
@@ -3033,7 +3055,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2">
       <c r="A33" s="14" t="s">
         <v>205</v>
       </c>
@@ -3041,35 +3063,35 @@
         <v>204</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2">
       <c r="B35" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2">
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2">
       <c r="B37" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2">
       <c r="B38" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2">
       <c r="B39" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2">
       <c r="B41" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2">
       <c r="B42" s="1" t="s">
         <v>230</v>
       </c>
@@ -3078,6 +3100,11 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3089,12 +3116,12 @@
       <selection activeCell="B38" sqref="B38:B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3123,7 +3150,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
         <v>130</v>
       </c>
@@ -3152,7 +3179,7 @@
         <v>41192</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9">
       <c r="A4" s="14" t="s">
         <v>220</v>
       </c>
@@ -3160,7 +3187,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="A5" s="14" t="s">
         <v>221</v>
       </c>
@@ -3168,7 +3195,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
         <v>136</v>
       </c>
@@ -3197,7 +3224,7 @@
         <v>41192</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9">
       <c r="A9" s="14" t="s">
         <v>212</v>
       </c>
@@ -3205,7 +3232,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="A10" s="14" t="s">
         <v>214</v>
       </c>
@@ -3213,7 +3240,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9">
       <c r="A13" s="4" t="s">
         <v>150</v>
       </c>
@@ -3242,7 +3269,7 @@
         <v>41193</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>224</v>
       </c>
@@ -3250,7 +3277,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>225</v>
       </c>
@@ -3258,7 +3285,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>228</v>
       </c>
@@ -3266,7 +3293,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9">
       <c r="A19" s="4" t="s">
         <v>152</v>
       </c>
@@ -3295,7 +3322,7 @@
         <v>41193</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>216</v>
       </c>
@@ -3303,7 +3330,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>218</v>
       </c>
@@ -3311,7 +3338,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9">
       <c r="A24" s="4" t="s">
         <v>116</v>
       </c>
@@ -3340,7 +3367,7 @@
         <v>41193</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>231</v>
       </c>
@@ -3348,7 +3375,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>234</v>
       </c>
@@ -3356,7 +3383,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>235</v>
       </c>
@@ -3364,7 +3391,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>236</v>
       </c>
@@ -3372,7 +3399,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9">
       <c r="A31" s="4" t="s">
         <v>124</v>
       </c>
@@ -3401,7 +3428,7 @@
         <v>41193</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>237</v>
       </c>
@@ -3409,7 +3436,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>241</v>
       </c>
@@ -3417,7 +3444,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>242</v>
       </c>
@@ -3425,7 +3452,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2" ht="26">
       <c r="A36" t="s">
         <v>243</v>
       </c>
@@ -3433,55 +3460,55 @@
         <v>239</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2">
       <c r="B38" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2">
       <c r="B40" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2">
       <c r="B41" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2">
       <c r="B42" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2">
       <c r="B43" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2" ht="26">
       <c r="B44" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2">
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2">
       <c r="B46" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2">
       <c r="B47" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2">
       <c r="B48" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:2">
       <c r="B49" s="1" t="s">
         <v>248</v>
       </c>
@@ -3490,6 +3517,11 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3497,16 +3529,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="B3" zoomScale="150" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="39.33203125" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3535,7 +3567,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
         <v>119</v>
       </c>
@@ -3564,10 +3596,10 @@
         <v>41206</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9">
       <c r="A4" s="14" t="s">
         <v>252</v>
       </c>
@@ -3575,7 +3607,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="A5" s="14" t="s">
         <v>253</v>
       </c>
@@ -3583,7 +3615,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9">
       <c r="A6" s="14" t="s">
         <v>254</v>
       </c>
@@ -3591,7 +3623,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9">
       <c r="A7" s="14" t="s">
         <v>258</v>
       </c>
@@ -3599,10 +3631,10 @@
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9">
       <c r="A8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
         <v>129</v>
       </c>
@@ -3631,7 +3663,7 @@
         <v>41194</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>259</v>
       </c>
@@ -3639,7 +3671,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>260</v>
       </c>
@@ -3647,7 +3679,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9">
       <c r="A14" s="4" t="s">
         <v>135</v>
       </c>
@@ -3676,7 +3708,7 @@
         <v>41203</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>282</v>
       </c>
@@ -3684,7 +3716,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>284</v>
       </c>
@@ -3692,7 +3724,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9">
       <c r="A18" s="4" t="s">
         <v>145</v>
       </c>
@@ -3721,7 +3753,7 @@
         <v>41203</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>286</v>
       </c>
@@ -3729,7 +3761,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>287</v>
       </c>
@@ -3737,7 +3769,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9">
       <c r="A23" s="4" t="s">
         <v>149</v>
       </c>
@@ -3766,7 +3798,7 @@
         <v>41203</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>273</v>
       </c>
@@ -3774,7 +3806,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>274</v>
       </c>
@@ -3782,7 +3814,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>275</v>
       </c>
@@ -3790,7 +3822,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9">
       <c r="A30" s="4" t="s">
         <v>153</v>
       </c>
@@ -3819,7 +3851,7 @@
         <v>41203</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>279</v>
       </c>
@@ -3827,7 +3859,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>280</v>
       </c>
@@ -3835,7 +3867,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>281</v>
       </c>
@@ -3843,60 +3875,60 @@
         <v>278</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2">
       <c r="B36" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2">
       <c r="B38" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2">
       <c r="B39" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2">
       <c r="B40" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2">
       <c r="B41" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2">
       <c r="B42" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2">
       <c r="B44" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2">
       <c r="B45" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2">
       <c r="B46" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2">
       <c r="B47" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2">
       <c r="B48" s="1" t="s">
         <v>318</v>
       </c>
@@ -3905,6 +3937,11 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3912,16 +3949,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A14" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3950,7 +3987,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
         <v>142</v>
       </c>
@@ -3979,7 +4016,7 @@
         <v>41207</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>263</v>
       </c>
@@ -3987,7 +4024,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>264</v>
       </c>
@@ -3995,7 +4032,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>265</v>
       </c>
@@ -4003,7 +4040,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
         <v>144</v>
       </c>
@@ -4032,7 +4069,7 @@
         <v>41206</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>268</v>
       </c>
@@ -4040,7 +4077,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>269</v>
       </c>
@@ -4048,7 +4085,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9">
       <c r="A13" s="4" t="s">
         <v>118</v>
       </c>
@@ -4068,7 +4105,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>290</v>
       </c>
@@ -4076,7 +4113,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>294</v>
       </c>
@@ -4084,7 +4121,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>295</v>
       </c>
@@ -4092,7 +4129,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9">
       <c r="A18" s="4" t="s">
         <v>120</v>
       </c>
@@ -4112,7 +4149,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>296</v>
       </c>
@@ -4120,7 +4157,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>300</v>
       </c>
@@ -4128,7 +4165,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>301</v>
       </c>
@@ -4136,7 +4173,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>302</v>
       </c>
@@ -4144,7 +4181,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9">
       <c r="A24" s="4" t="s">
         <v>138</v>
       </c>
@@ -4155,7 +4192,7 @@
         <v>160</v>
       </c>
       <c r="D24" t="s">
-        <v>251</v>
+        <v>211</v>
       </c>
       <c r="E24">
         <v>35</v>
@@ -4163,8 +4200,17 @@
       <c r="F24">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G24">
+        <v>19</v>
+      </c>
+      <c r="H24">
+        <v>15</v>
+      </c>
+      <c r="I24" s="17">
+        <v>41213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>312</v>
       </c>
@@ -4172,7 +4218,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>313</v>
       </c>
@@ -4180,7 +4226,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>314</v>
       </c>
@@ -4188,7 +4234,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>315</v>
       </c>
@@ -4196,7 +4242,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9">
       <c r="A33" s="4" t="s">
         <v>139</v>
       </c>
@@ -4207,7 +4253,7 @@
         <v>160</v>
       </c>
       <c r="D33" t="s">
-        <v>251</v>
+        <v>211</v>
       </c>
       <c r="E33">
         <v>35</v>
@@ -4215,8 +4261,17 @@
       <c r="F33">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G33">
+        <v>18</v>
+      </c>
+      <c r="H33">
+        <v>17</v>
+      </c>
+      <c r="I33" s="17">
+        <v>41213</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>304</v>
       </c>
@@ -4224,7 +4279,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>305</v>
       </c>
@@ -4232,7 +4287,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>306</v>
       </c>
@@ -4240,7 +4295,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>307</v>
       </c>
@@ -4252,6 +4307,11 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4263,13 +4323,13 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>114</v>
       </c>
@@ -4283,7 +4343,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="30">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -4297,7 +4357,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -4311,7 +4371,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -4325,7 +4385,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -4336,7 +4396,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -4350,7 +4410,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="15">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -4361,7 +4421,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="45">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -4375,7 +4435,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="30">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -4386,7 +4446,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="30">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -4397,7 +4457,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -4411,7 +4471,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="15">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -4422,7 +4482,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="48" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -4433,7 +4493,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="30">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -4444,7 +4504,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="15">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -4455,7 +4515,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="15">
       <c r="A16" t="s">
         <v>129</v>
       </c>
@@ -4469,7 +4529,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="15">
       <c r="A17" t="s">
         <v>130</v>
       </c>
@@ -4483,7 +4543,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15">
       <c r="A18" t="s">
         <v>131</v>
       </c>
@@ -4494,7 +4554,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15">
       <c r="A19" t="s">
         <v>132</v>
       </c>
@@ -4505,7 +4565,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -4516,7 +4576,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="15">
       <c r="A21" t="s">
         <v>134</v>
       </c>
@@ -4527,7 +4587,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="30">
       <c r="A22" t="s">
         <v>135</v>
       </c>
@@ -4538,7 +4598,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="30">
       <c r="A23" t="s">
         <v>136</v>
       </c>
@@ -4552,7 +4612,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="30">
       <c r="A24" t="s">
         <v>137</v>
       </c>
@@ -4566,7 +4626,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="48" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="30">
       <c r="A25" t="s">
         <v>138</v>
       </c>
@@ -4577,7 +4637,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="30">
       <c r="A26" t="s">
         <v>139</v>
       </c>
@@ -4588,7 +4648,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="80" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="60">
       <c r="A27" t="s">
         <v>140</v>
       </c>
@@ -4599,7 +4659,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15">
       <c r="A28" t="s">
         <v>141</v>
       </c>
@@ -4613,7 +4673,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="15">
       <c r="A29" t="s">
         <v>142</v>
       </c>
@@ -4627,7 +4687,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="15">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -4641,7 +4701,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="15">
       <c r="A31" t="s">
         <v>144</v>
       </c>
@@ -4655,7 +4715,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="30">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -4666,7 +4726,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="15">
       <c r="A33" t="s">
         <v>146</v>
       </c>
@@ -4677,7 +4737,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="30">
       <c r="A34" t="s">
         <v>147</v>
       </c>
@@ -4688,7 +4748,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="48" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="30">
       <c r="A35" t="s">
         <v>148</v>
       </c>
@@ -4699,7 +4759,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="30">
       <c r="A36" t="s">
         <v>149</v>
       </c>
@@ -4710,7 +4770,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="15">
       <c r="A37" t="s">
         <v>150</v>
       </c>
@@ -4724,7 +4784,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="30">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -4735,7 +4795,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="30">
       <c r="A39" t="s">
         <v>152</v>
       </c>
@@ -4749,7 +4809,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="30">
       <c r="A40" t="s">
         <v>153</v>
       </c>
@@ -4760,7 +4820,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="30">
       <c r="A41" t="s">
         <v>154</v>
       </c>
@@ -4771,7 +4831,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="15">
       <c r="A42" t="s">
         <v>155</v>
       </c>
@@ -4782,7 +4842,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="30">
       <c r="A43" t="s">
         <v>156</v>
       </c>
@@ -4796,5 +4856,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Report updated and US04 and US06 added
</commit_message>
<xml_diff>
--- a/Team Report_Rafif, Maha, Saloni-Final.xlsx
+++ b/Team Report_Rafif, Maha, Saloni-Final.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27610"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafifarab/Desktop/SSW-555-GEDCOM/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -16,20 +21,20 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId7"/>
     <sheet name="Stories" sheetId="11" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="318">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -813,9 +818,6 @@
   </si>
   <si>
     <t>y</t>
-  </si>
-  <si>
-    <t>Initiated</t>
   </si>
   <si>
     <t>T05.01</t>
@@ -1398,6 +1400,9 @@
                 <c:pt idx="3">
                   <c:v>41213.0</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>41227.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1419,6 +1424,9 @@
                 <c:pt idx="3">
                   <c:v>24.0</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1434,11 +1442,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2096541624"/>
-        <c:axId val="-2096624280"/>
+        <c:axId val="-1998719008"/>
+        <c:axId val="-1999210464"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2096541624"/>
+        <c:axId val="-1998719008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,14 +1456,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096624280"/>
+        <c:crossAx val="-1999210464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2096624280"/>
+        <c:axId val="-1999210464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1466,7 +1474,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096541624"/>
+        <c:crossAx val="-1998719008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1844,15 +1852,15 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="5" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -1869,7 +1877,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>159</v>
       </c>
@@ -1886,7 +1894,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>160</v>
       </c>
@@ -1900,10 +1908,10 @@
         <v>167</v>
       </c>
       <c r="E4" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -1920,7 +1928,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>29</v>
       </c>
@@ -1940,11 +1948,6 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1952,20 +1955,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>208</v>
       </c>
@@ -1982,7 +1985,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2016,7 +2019,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2033,7 +2036,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2047,10 +2050,10 @@
         <v>159</v>
       </c>
       <c r="E5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2067,7 +2070,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2081,10 +2084,10 @@
         <v>159</v>
       </c>
       <c r="E7" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>122</v>
       </c>
@@ -2109,7 +2112,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>123</v>
       </c>
@@ -2117,7 +2120,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2134,7 +2137,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>125</v>
       </c>
@@ -2142,7 +2145,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>126</v>
       </c>
@@ -2150,7 +2153,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>127</v>
       </c>
@@ -2158,7 +2161,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>128</v>
       </c>
@@ -2166,7 +2169,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2183,7 +2186,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2200,7 +2203,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>131</v>
       </c>
@@ -2208,7 +2211,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>132</v>
       </c>
@@ -2216,7 +2219,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>133</v>
       </c>
@@ -2224,7 +2227,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>134</v>
       </c>
@@ -2232,7 +2235,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2249,7 +2252,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2266,7 +2269,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2283,7 +2286,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>4</v>
       </c>
@@ -2300,7 +2303,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>4</v>
       </c>
@@ -2317,7 +2320,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
         <v>140</v>
       </c>
@@ -2325,7 +2328,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>4</v>
       </c>
@@ -2359,7 +2362,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2376,7 +2379,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2410,7 +2413,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B33" t="s">
         <v>146</v>
       </c>
@@ -2418,7 +2421,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B34" t="s">
         <v>147</v>
       </c>
@@ -2426,7 +2429,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B35" t="s">
         <v>148</v>
       </c>
@@ -2434,7 +2437,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2451,7 +2454,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>2</v>
       </c>
@@ -2468,7 +2471,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B38" t="s">
         <v>151</v>
       </c>
@@ -2476,7 +2479,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>2</v>
       </c>
@@ -2493,7 +2496,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2510,7 +2513,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B41" t="s">
         <v>154</v>
       </c>
@@ -2518,7 +2521,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B42" t="s">
         <v>155</v>
       </c>
@@ -2526,7 +2529,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B43" t="s">
         <v>156</v>
       </c>
@@ -2538,33 +2541,28 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="2"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2584,7 +2582,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>41171</v>
       </c>
@@ -2604,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>41185</v>
       </c>
@@ -2626,7 +2624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>41193</v>
       </c>
@@ -2648,7 +2646,7 @@
         <v>9.5192307692307683</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="6">
         <v>41213</v>
       </c>
@@ -2667,6 +2665,27 @@
       <c r="F5" s="8">
         <f>(D5-D4)/E5*60</f>
         <v>17.202797202797203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="2">
+        <v>41227</v>
+      </c>
+      <c r="B6">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>128</v>
+      </c>
+      <c r="E6">
+        <v>96</v>
+      </c>
+      <c r="F6" s="8">
+        <f>(D5-D6)/E6*60</f>
+        <v>31.250000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -2674,11 +2693,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2690,21 +2704,21 @@
       <selection activeCell="H30" sqref="H2:H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="6"/>
-    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="6"/>
+    <col min="11" max="11" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2733,7 +2747,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>115</v>
       </c>
@@ -2762,10 +2776,10 @@
         <v>41182</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>182</v>
       </c>
@@ -2773,7 +2787,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>183</v>
       </c>
@@ -2781,10 +2795,10 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="14"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>117</v>
       </c>
@@ -2813,10 +2827,10 @@
         <v>41184</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>176</v>
       </c>
@@ -2824,7 +2838,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -2832,7 +2846,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>180</v>
       </c>
@@ -2840,7 +2854,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>121</v>
       </c>
@@ -2869,11 +2883,11 @@
         <v>41181</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
         <v>186</v>
       </c>
@@ -2881,7 +2895,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
         <v>187</v>
       </c>
@@ -2889,7 +2903,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="26">
+    <row r="17" spans="1:9" ht="39" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
         <v>198</v>
       </c>
@@ -2897,7 +2911,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="26">
+    <row r="18" spans="1:9" ht="39" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
         <v>199</v>
       </c>
@@ -2905,10 +2919,10 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>137</v>
       </c>
@@ -2937,11 +2951,11 @@
         <v>41184</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="14" t="s">
         <v>193</v>
       </c>
@@ -2949,7 +2963,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="14" t="s">
         <v>194</v>
       </c>
@@ -2957,7 +2971,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="26">
+    <row r="24" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A24" s="14" t="s">
         <v>195</v>
       </c>
@@ -2965,11 +2979,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>141</v>
       </c>
@@ -2998,11 +3012,11 @@
         <v>41184</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="4"/>
       <c r="B27"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="14" t="s">
         <v>189</v>
       </c>
@@ -3010,11 +3024,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="14"/>
       <c r="B29"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>143</v>
       </c>
@@ -3043,11 +3057,11 @@
         <v>41184</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="4"/>
       <c r="B31"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="14" t="s">
         <v>202</v>
       </c>
@@ -3055,7 +3069,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="14" t="s">
         <v>205</v>
       </c>
@@ -3063,35 +3077,35 @@
         <v>204</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B35" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B37" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B38" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B41" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
         <v>230</v>
       </c>
@@ -3100,11 +3114,6 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3116,12 +3125,12 @@
       <selection activeCell="B38" sqref="B38:B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3150,7 +3159,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>130</v>
       </c>
@@ -3179,7 +3188,7 @@
         <v>41192</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>220</v>
       </c>
@@ -3187,7 +3196,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>221</v>
       </c>
@@ -3195,7 +3204,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>136</v>
       </c>
@@ -3224,7 +3233,7 @@
         <v>41192</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>212</v>
       </c>
@@ -3232,7 +3241,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
         <v>214</v>
       </c>
@@ -3240,7 +3249,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>150</v>
       </c>
@@ -3269,7 +3278,7 @@
         <v>41193</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>224</v>
       </c>
@@ -3277,7 +3286,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>225</v>
       </c>
@@ -3285,7 +3294,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>228</v>
       </c>
@@ -3293,7 +3302,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>152</v>
       </c>
@@ -3322,7 +3331,7 @@
         <v>41193</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>216</v>
       </c>
@@ -3330,7 +3339,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>218</v>
       </c>
@@ -3338,7 +3347,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>116</v>
       </c>
@@ -3367,7 +3376,7 @@
         <v>41193</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>231</v>
       </c>
@@ -3375,7 +3384,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>234</v>
       </c>
@@ -3383,7 +3392,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>235</v>
       </c>
@@ -3391,7 +3400,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>236</v>
       </c>
@@ -3399,7 +3408,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>124</v>
       </c>
@@ -3428,7 +3437,7 @@
         <v>41193</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>237</v>
       </c>
@@ -3436,7 +3445,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>241</v>
       </c>
@@ -3444,7 +3453,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>242</v>
       </c>
@@ -3452,7 +3461,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="26">
+    <row r="36" spans="1:2" ht="26" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>243</v>
       </c>
@@ -3460,55 +3469,55 @@
         <v>239</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B38" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B40" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B41" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="26">
+    <row r="44" spans="1:2" ht="26" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B46" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B48" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="49" spans="2:2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
         <v>248</v>
       </c>
@@ -3517,11 +3526,6 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3533,12 +3537,12 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="39.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3567,7 +3571,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>119</v>
       </c>
@@ -3596,45 +3600,45 @@
         <v>41206</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" s="14" t="s">
         <v>252</v>
-      </c>
-      <c r="B4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="14" t="s">
-        <v>253</v>
       </c>
       <c r="B5" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="B7" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="B7" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="14"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>129</v>
       </c>
@@ -3663,23 +3667,23 @@
         <v>41194</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
         <v>259</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>260</v>
-      </c>
-      <c r="B12" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>135</v>
       </c>
@@ -3708,23 +3712,23 @@
         <v>41203</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
+        <v>281</v>
+      </c>
+      <c r="B15" t="s">
         <v>282</v>
       </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>284</v>
       </c>
-      <c r="B16" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>145</v>
       </c>
@@ -3753,23 +3757,23 @@
         <v>41203</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
+        <v>285</v>
+      </c>
+      <c r="B19" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
         <v>286</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
-        <v>287</v>
-      </c>
-      <c r="B20" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>149</v>
       </c>
@@ -3798,31 +3802,31 @@
         <v>41203</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
+        <v>272</v>
+      </c>
+      <c r="B25" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
         <v>273</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
         <v>274</v>
-      </c>
-      <c r="B26" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" t="s">
-        <v>275</v>
       </c>
       <c r="B27" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>153</v>
       </c>
@@ -3851,97 +3855,92 @@
         <v>41203</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
+        <v>278</v>
+      </c>
+      <c r="B32" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
         <v>279</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
         <v>280</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>281</v>
-      </c>
-      <c r="B34" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B38" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B41" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B42" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="B42" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B44" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" ht="26" x14ac:dyDescent="0.15">
       <c r="B48" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3949,16 +3948,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3987,7 +3986,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>142</v>
       </c>
@@ -4016,31 +4015,31 @@
         <v>41207</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>262</v>
+      </c>
+      <c r="B4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>263</v>
-      </c>
-      <c r="B4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>264</v>
       </c>
       <c r="B5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B6" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>144</v>
       </c>
@@ -4069,23 +4068,23 @@
         <v>41206</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
+        <v>267</v>
+      </c>
+      <c r="B10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
         <v>268</v>
       </c>
-      <c r="B10" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>269</v>
       </c>
-      <c r="B11" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>118</v>
       </c>
@@ -4096,7 +4095,7 @@
         <v>159</v>
       </c>
       <c r="D13" t="s">
-        <v>251</v>
+        <v>211</v>
       </c>
       <c r="E13">
         <v>30</v>
@@ -4104,32 +4103,41 @@
       <c r="F13">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="G13">
+        <v>25</v>
+      </c>
+      <c r="H13">
+        <v>7</v>
+      </c>
+      <c r="I13" s="17">
+        <v>41216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
+        <v>289</v>
+      </c>
+      <c r="B14" t="s">
         <v>290</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>293</v>
+      </c>
+      <c r="B15" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
         <v>294</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>295</v>
-      </c>
-      <c r="B16" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>120</v>
       </c>
@@ -4140,7 +4148,7 @@
         <v>159</v>
       </c>
       <c r="D18" t="s">
-        <v>251</v>
+        <v>211</v>
       </c>
       <c r="E18">
         <v>30</v>
@@ -4148,40 +4156,49 @@
       <c r="F18">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="G18">
+        <v>24</v>
+      </c>
+      <c r="H18">
+        <v>7</v>
+      </c>
+      <c r="I18" s="17">
+        <v>41216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B19" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
+        <v>299</v>
+      </c>
+      <c r="B20" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
         <v>300</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
         <v>301</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" t="s">
-        <v>302</v>
-      </c>
-      <c r="B22" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>138</v>
       </c>
@@ -4210,39 +4227,39 @@
         <v>41213</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
+        <v>311</v>
+      </c>
+      <c r="B26" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
         <v>312</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
         <v>313</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
         <v>314</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" t="s">
-        <v>315</v>
-      </c>
-      <c r="B29" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>139</v>
       </c>
@@ -4271,47 +4288,42 @@
         <v>41213</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
+        <v>303</v>
+      </c>
+      <c r="B35" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
         <v>304</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
-      <c r="A36" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
         <v>305</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
-      <c r="A37" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
         <v>306</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>310</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
-        <v>307</v>
-      </c>
-      <c r="B38" t="s">
-        <v>311</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4323,13 +4335,13 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>114</v>
       </c>
@@ -4343,7 +4355,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -4357,7 +4369,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -4371,7 +4383,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -4385,7 +4397,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30">
+    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -4396,7 +4408,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -4410,7 +4422,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -4421,7 +4433,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45">
+    <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -4435,7 +4447,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30">
+    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -4446,7 +4458,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30">
+    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -4457,7 +4469,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15">
+    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -4471,7 +4483,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15">
+    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -4482,7 +4494,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30">
+    <row r="13" spans="1:4" ht="48" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -4493,7 +4505,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30">
+    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -4504,7 +4516,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15">
+    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -4515,7 +4527,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>129</v>
       </c>
@@ -4529,7 +4541,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15">
+    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>130</v>
       </c>
@@ -4543,7 +4555,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>131</v>
       </c>
@@ -4554,7 +4566,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>132</v>
       </c>
@@ -4565,7 +4577,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -4576,7 +4588,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15">
+    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>134</v>
       </c>
@@ -4587,7 +4599,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30">
+    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>135</v>
       </c>
@@ -4598,7 +4610,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30">
+    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>136</v>
       </c>
@@ -4612,7 +4624,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30">
+    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>137</v>
       </c>
@@ -4626,7 +4638,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30">
+    <row r="25" spans="1:4" ht="48" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>138</v>
       </c>
@@ -4637,7 +4649,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30">
+    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>139</v>
       </c>
@@ -4648,7 +4660,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="60">
+    <row r="27" spans="1:4" ht="80" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>140</v>
       </c>
@@ -4659,7 +4671,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15">
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>141</v>
       </c>
@@ -4673,7 +4685,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15">
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>142</v>
       </c>
@@ -4687,7 +4699,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -4701,7 +4713,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>144</v>
       </c>
@@ -4715,7 +4727,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30">
+    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -4726,7 +4738,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15">
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>146</v>
       </c>
@@ -4737,7 +4749,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30">
+    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>147</v>
       </c>
@@ -4748,7 +4760,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30">
+    <row r="35" spans="1:4" ht="48" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>148</v>
       </c>
@@ -4759,7 +4771,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30">
+    <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>149</v>
       </c>
@@ -4770,7 +4782,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15">
+    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>150</v>
       </c>
@@ -4784,7 +4796,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30">
+    <row r="38" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -4795,7 +4807,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30">
+    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>152</v>
       </c>
@@ -4809,7 +4821,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30">
+    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>153</v>
       </c>
@@ -4820,7 +4832,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30">
+    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>154</v>
       </c>
@@ -4831,7 +4843,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15">
+    <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>155</v>
       </c>
@@ -4842,7 +4854,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30">
+    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>156</v>
       </c>
@@ -4856,10 +4868,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>